<commit_message>
Ajuste do código da develop para rodar a Build. Ainda são necessários ajustes nos StructuresDefinitions e conserto do que é apontado em qa.html
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-BRIndividuo-1.0.xlsx
+++ b/output/StructureDefinition-BRIndividuo-1.0.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-22T19:20:27-03:00</t>
+    <t>2024-10-10T15:46:28-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1579,7 +1579,7 @@
     <t>Distinguishes between physical addresses (those you can visit) and mailing addresses (e.g. PO Boxes and care-of addresses). Most addresses are both.</t>
   </si>
   <si>
-    <t>The definition of Address states that "address is intended to describe postal addresses, not physical locations". However, many applications track whether an address has a dual purpose of being a location that can be visited as well as being a valid delivery destination, and Postal addresses are often used as proxies for physical locations (also see the [Location](location.html#) resource).</t>
+    <t>The definition of Address states that "address is intended to describe postal addresses, not physical locations". However, many applications track whether an address has a dual purpose of being a location that can be visited as well as being a valid delivery destination, and Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
   </si>
   <si>
     <t>both</t>
@@ -2596,15 +2596,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="53.9296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.296875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.27734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="51.6953125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="37.484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.8203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="37.5859375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.47265625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.87890625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.2734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.7265625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2615,27 +2615,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="52.28125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="36.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.4609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.86328125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="91.51171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="49.3671875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.52734375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="38.34375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.06640625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.421875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="32.73046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.28515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.6875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="153.5546875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="39.8515625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="102.75390625" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="35.6015625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="147.8359375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="38.20703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="32.4453125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="98.66796875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="35.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>